<commit_message>
Corregir error de referencia en la celda de exportación a Excel en lead_scoring_openai.ipynb
</commit_message>
<xml_diff>
--- a/leads_analizados.xlsx
+++ b/leads_analizados.xlsx
@@ -822,11 +822,11 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>🔴 Frío</t>
+          <t>🟡 Tibio</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">

</xml_diff>

<commit_message>
Agregar validación de clave API, mejorar manejo de errores y optimizar la descarga de archivos en la aplicación de puntuación de leads
</commit_message>
<xml_diff>
--- a/leads_analizados.xlsx
+++ b/leads_analizados.xlsx
@@ -822,11 +822,11 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>🟡 Tibio</t>
+          <t>🔴 Frío</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">

</xml_diff>

<commit_message>
Actualizar archivo de leads analizados
</commit_message>
<xml_diff>
--- a/leads_analizados.xlsx
+++ b/leads_analizados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,12 +501,10 @@
           <t>Estoy interesada en crear una tienda online para vender productos sostenibles.</t>
         </is>
       </c>
-      <c r="F2" t="n">
-        <v>5</v>
-      </c>
+      <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
-          <t>🟢 Caliente</t>
+          <t>❓</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -518,115 +516,109 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Luis</t>
+          <t>Carla</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>luis@email.com</t>
+          <t>carla@email.com</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Comercial Luis</t>
+          <t>Studio Creativo</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>mediana</t>
+          <t>pequeña</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Necesito urgentemente una solución de stock y un ecommerce funcional.</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>5</v>
-      </c>
+          <t>Solo estoy viendo opciones por ahora quiero saber precios.</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
-          <t>🟢 Caliente</t>
+          <t>❓</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>E-commerce</t>
+          <t>Otro</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Carla</t>
+          <t>Mario</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>carla@email.com</t>
+          <t>mario@email.com</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Studio Creativo</t>
+          <t>Mario Consulting</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>pequeña</t>
+          <t>grande</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Solo estoy viendo opciones por ahora quiero saber precios.</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>3</v>
-      </c>
+          <t>Busco rediseñar mi sitio web y conectar con redes sociales.</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
-          <t>🟡 Tibio</t>
+          <t>❓</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Otro</t>
+          <t>Sitio Web</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Mario</t>
+          <t>Lucía</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>mario@email.com</t>
+          <t>lucia@email.com</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Mario Consulting</t>
+          <t>Lucía Fit</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>grande</t>
+          <t>pequeña</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Busco rediseñar mi sitio web y conectar con redes sociales.</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>5</v>
-      </c>
+          <t>Me interesa una página web simple para mis clases online.</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
-          <t>🟢 Caliente</t>
+          <t>❓</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -638,35 +630,33 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Lucía</t>
+          <t>Juan</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>lucia@email.com</t>
+          <t>juan@email.com</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Lucía Fit</t>
+          <t>Distribuidora Juan</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>pequeña</t>
+          <t>mediana</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Me interesa una página web simple para mis clases online.</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>4</v>
-      </c>
+          <t>Realizan aplicaciones web?.</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
         <is>
-          <t>🟢 Caliente</t>
+          <t>❓</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -678,57 +668,55 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Juan</t>
+          <t>Cecilia</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>juan@email.com</t>
+          <t>cecilia@email.com</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Distribuidora Juan</t>
+          <t>CeMarket</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>mediana</t>
+          <t>grande</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Tengo presupuesto aprobado para crear un ecommerce personalizado.</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>5</v>
-      </c>
+          <t>Estoy interesada en SEO local y visibilidad en Google Maps.</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr">
         <is>
-          <t>🟢 Caliente</t>
+          <t>❓</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>E-commerce</t>
+          <t>Otro</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Sofía</t>
+          <t>Iván</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>sofia@email.com</t>
+          <t>ivan@email.com</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Redes Pro</t>
+          <t>Shopify Partners</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -738,218 +726,54 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Quiero mejorar mi perfil de Instagram y tener una landing para captar leads.</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>5</v>
-      </c>
+          <t>Quiero conectar mi tienda Shopify con WhatsApp para soporte.</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr">
         <is>
-          <t>🟢 Caliente</t>
+          <t>❓</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Redes Sociales</t>
+          <t>E-commerce</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Pedro</t>
+          <t>Alicia</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>pedro@email.com</t>
+          <t>alicia@email.com</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Eventos Pedro</t>
+          <t>Alimarket</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>pequeña</t>
+          <t>mediana</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Quiero saber si ofrecen consultoría o solo diseño web.</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
-        <v>4</v>
-      </c>
+          <t>Quiero lanzar mi tienda en un marketplace y necesito asesoría.</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr">
         <is>
-          <t>🟢 Caliente</t>
+          <t>❓</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
-        <is>
-          <t>Sitio Web</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Marta</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>marta@email.com</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Marta Yoga</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>pequeña</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Quiero una web bonita pero no tengo prisa ni presupuesto ahora.</t>
-        </is>
-      </c>
-      <c r="F10" t="n">
-        <v>2</v>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>🔴 Frío</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>Sitio Web</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Raúl</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>raul@email.com</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>R-Tech</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>grande</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Necesitamos migrar todo nuestro sistema de ventas a una plataforma digital escalable.</t>
-        </is>
-      </c>
-      <c r="F11" t="n">
-        <v>5</v>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>🟢 Caliente</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>Otro</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Claudia</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>claudia@email.com</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Clau Social</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>pequeña</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Busco a alguien que gestione campañas en redes y SEO básico.</t>
-        </is>
-      </c>
-      <c r="F12" t="n">
-        <v>4</v>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>🟢 Caliente</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>Redes Sociales</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Esteban</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>esteban@email.com</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Importaciones Este</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>grande</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Estoy cotizando varias agencias y quiero ver ejemplos de ecommerce.</t>
-        </is>
-      </c>
-      <c r="F13" t="n">
-        <v>4</v>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>🟢 Caliente</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
         <is>
           <t>E-commerce</t>
         </is>

</xml_diff>